<commit_message>
Adding support for sheets.
</commit_message>
<xml_diff>
--- a/ExcelEnumerable.Tests/Example.xlsx
+++ b/ExcelEnumerable.Tests/Example.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27720" windowHeight="12450"/>
+    <workbookView windowWidth="24000" windowHeight="10155" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Another Sheet" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>First Name</t>
   </si>
@@ -56,6 +57,21 @@
   </si>
   <si>
     <t>Final Address 22</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Las Vegas</t>
   </si>
 </sst>
 </file>
@@ -63,11 +79,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -88,14 +104,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -109,15 +117,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -133,6 +135,52 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -140,7 +188,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -149,14 +197,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -178,30 +218,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -214,7 +231,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -231,85 +247,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -321,97 +415,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -425,65 +441,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -514,6 +476,60 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -527,142 +543,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="7" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1000,8 +1016,8 @@
   <sheetPr/>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75" outlineLevelRow="3" outlineLevelCol="4"/>
@@ -1082,4 +1098,46 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75" outlineLevelRow="4"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding support for sheets. (#13)
</commit_message>
<xml_diff>
--- a/ExcelEnumerable.Tests/Example.xlsx
+++ b/ExcelEnumerable.Tests/Example.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27720" windowHeight="12450"/>
+    <workbookView windowWidth="24000" windowHeight="10155" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Another Sheet" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>First Name</t>
   </si>
@@ -56,6 +57,21 @@
   </si>
   <si>
     <t>Final Address 22</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Las Vegas</t>
   </si>
 </sst>
 </file>
@@ -63,11 +79,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -88,14 +104,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -109,15 +117,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -133,6 +135,52 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -140,7 +188,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -149,14 +197,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -178,30 +218,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -214,7 +231,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -231,85 +247,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -321,97 +415,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -425,65 +441,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -514,6 +476,60 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -527,142 +543,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="7" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1000,8 +1016,8 @@
   <sheetPr/>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75" outlineLevelRow="3" outlineLevelCol="4"/>
@@ -1082,4 +1098,46 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75" outlineLevelRow="4"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Version 2 without complete tests
</commit_message>
<xml_diff>
--- a/ExcelEnumerable.Tests/Example.xlsx
+++ b/ExcelEnumerable.Tests/Example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24000" windowHeight="10155" activeTab="1"/>
+    <workbookView windowWidth="24000" windowHeight="10155"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>First Name</t>
   </si>
@@ -41,6 +41,9 @@
     <t>Sample Address 11</t>
   </si>
   <si>
+    <t>t</t>
+  </si>
+  <si>
     <t>Another</t>
   </si>
   <si>
@@ -48,6 +51,9 @@
   </si>
   <si>
     <t>Testing Address 33</t>
+  </si>
+  <si>
+    <t>f</t>
   </si>
   <si>
     <t>Some</t>
@@ -79,11 +85,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="dd/mm/yyyy;@"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -103,7 +109,54 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -117,6 +170,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,114 +192,53 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -247,37 +253,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -289,7 +403,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -301,133 +421,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -441,21 +447,25 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -476,17 +486,37 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -514,171 +544,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="7" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1016,8 +1022,8 @@
   <sheetPr/>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75" outlineLevelRow="3" outlineLevelCol="4"/>
@@ -1056,42 +1062,42 @@
       <c r="D2" s="1">
         <v>32939</v>
       </c>
-      <c r="E2" t="b">
-        <v>1</v>
+      <c r="E2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1">
         <v>21186</v>
       </c>
-      <c r="E3" t="b">
-        <v>0</v>
+      <c r="E3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1">
         <v>41215</v>
       </c>
-      <c r="E4" t="b">
-        <v>1</v>
+      <c r="E4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1105,7 +1111,7 @@
   <sheetPr/>
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -1113,27 +1119,27 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>